<commit_message>
per HCD inspector requests 4/28
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\PycharmProjects\HCDpdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976DDD4D-2EAD-4920-8644-2F21E05387F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8659FD2E-BE3C-47FE-877B-3F32E29FC96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A73F84BD-3259-49CC-9357-80230FC0B03D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{A73F84BD-3259-49CC-9357-80230FC0B03D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="88">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -79,21 +79,6 @@
     <t>has to be date format</t>
   </si>
   <si>
-    <t>Seaview</t>
-  </si>
-  <si>
-    <t>LBK2086</t>
-  </si>
-  <si>
-    <t>blah</t>
-  </si>
-  <si>
-    <t>Hitching Post</t>
-  </si>
-  <si>
-    <t>Hitching Post Mobile Home Park LLC</t>
-  </si>
-  <si>
     <t>ie) Hitching Post Mobile Home Park LLC, carrier -- Victor Chen</t>
   </si>
   <si>
@@ -109,18 +94,12 @@
     <t>ie) last first middle</t>
   </si>
   <si>
-    <t>Campbell Timothy</t>
-  </si>
-  <si>
     <t>prevaddress</t>
   </si>
   <si>
     <t>address of previous owner (found on title)</t>
   </si>
   <si>
-    <t>398 E 21st, Costa Mesa CA</t>
-  </si>
-  <si>
     <t>date that coach was "sold" to you (just put 3 months prior)</t>
   </si>
   <si>
@@ -136,44 +115,202 @@
     <t>make sure to make this a string, exactly formatted " 'Jan 01, 1990"</t>
   </si>
   <si>
-    <t>Jan 01, 1990</t>
-  </si>
-  <si>
-    <t>Jun 04, 2022</t>
-  </si>
-  <si>
-    <t>Apr 15, 2022</t>
-  </si>
-  <si>
     <t>*Red means: do not alter (hard coded into the fabric of the cooooode</t>
   </si>
   <si>
     <t>spellpurchaseprice</t>
   </si>
   <si>
+    <t>ie) zero</t>
+  </si>
+  <si>
+    <t>ie) Hitching Post ("Mobile Home Park" will be appended auto)</t>
+  </si>
+  <si>
+    <t>ie) 34184 county line rd, sp #54 ("Yucaipa, CA 92399" will be appended auto)</t>
+  </si>
+  <si>
     <t>zero</t>
   </si>
   <si>
-    <t>ie) zero</t>
-  </si>
-  <si>
-    <t>ie) Hitching Post ("Mobile Home Park" will be appended auto)</t>
-  </si>
-  <si>
-    <t>ie) 34184 county line rd, sp #54 ("Yucaipa, CA 92399" will be appended auto)</t>
-  </si>
-  <si>
-    <t>34642 Yucaipa Blvd, Sp #10</t>
+    <t>buyer_name</t>
+  </si>
+  <si>
+    <t>buyer_phone</t>
+  </si>
+  <si>
+    <t>buyer_address</t>
+  </si>
+  <si>
+    <t>909 816 3161</t>
+  </si>
+  <si>
+    <t>Walter Watson</t>
+  </si>
+  <si>
+    <t>Aladdin Mobile Home Park</t>
+  </si>
+  <si>
+    <t>LBI5715</t>
+  </si>
+  <si>
+    <t>S1117</t>
+  </si>
+  <si>
+    <t>Aladdin</t>
+  </si>
+  <si>
+    <t>33562 Yucaipa Blvd, St 4-237, Yucaipa CA 92399</t>
+  </si>
+  <si>
+    <t>Rivera</t>
+  </si>
+  <si>
+    <t>LBK9663</t>
+  </si>
+  <si>
+    <t>R571X11FD1410</t>
+  </si>
+  <si>
+    <t>A36550</t>
+  </si>
+  <si>
+    <t>Putnam Family Partnership</t>
+  </si>
+  <si>
+    <t>Avalon</t>
+  </si>
+  <si>
+    <t>Cascade</t>
+  </si>
+  <si>
+    <t>LBI6352</t>
+  </si>
+  <si>
+    <t>S2140</t>
+  </si>
+  <si>
+    <t>D0HA49942</t>
+  </si>
+  <si>
+    <t>Lancer</t>
+  </si>
+  <si>
+    <t>Jan 1, 1963</t>
+  </si>
+  <si>
+    <t>35011 Avenue E, Sp 10, Yucaipa CA, 92399</t>
+  </si>
+  <si>
+    <t>Avalon Mobile Home Park</t>
+  </si>
+  <si>
+    <t>Apr 13, 2023</t>
+  </si>
+  <si>
+    <t>Avalon 10</t>
+  </si>
+  <si>
+    <t>Jan 1, 1962</t>
+  </si>
+  <si>
+    <t>35011 Avenue E, Sp 9, Yucaipa CA, 92399</t>
+  </si>
+  <si>
+    <t>Avalon 9</t>
+  </si>
+  <si>
+    <t>Aladdin 16</t>
+  </si>
+  <si>
+    <t>Dec 12, 1969</t>
+  </si>
+  <si>
+    <t>12813 7th St, Sp 16, Yucaipa CA, 92399</t>
+  </si>
+  <si>
+    <t>Mary Watson</t>
+  </si>
+  <si>
+    <t>Apr 27, 2023</t>
+  </si>
+  <si>
+    <t>Kaufman/Broad</t>
+  </si>
+  <si>
+    <t>Jan 1, 1980</t>
+  </si>
+  <si>
+    <t>LAH4140</t>
+  </si>
+  <si>
+    <t>KBCASNA015388/KBCASNB015388</t>
+  </si>
+  <si>
+    <t>CAL190907/CAL190908</t>
+  </si>
+  <si>
+    <t>13063 5th St, Sp 10, Yucaipa CA, 92399</t>
+  </si>
+  <si>
+    <t>Wishing Well</t>
+  </si>
+  <si>
+    <t>Wishing Well Mobile Home Park, LLC</t>
+  </si>
+  <si>
+    <t>Cornish Construction Co</t>
+  </si>
+  <si>
+    <t>PO Box 359, Bloomington CA 92316</t>
+  </si>
+  <si>
+    <t>Mar 14, 2022</t>
+  </si>
+  <si>
+    <t>blankfornow</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+  <si>
+    <t>applicantname</t>
+  </si>
+  <si>
+    <t>Victor Chen</t>
+  </si>
+  <si>
+    <t>ie) Victor Chen</t>
+  </si>
+  <si>
+    <t>descr_of_work1</t>
+  </si>
+  <si>
+    <t>water heater, AC packaged unit (no suctions), new cabinets, new sink, new toilet</t>
+  </si>
+  <si>
+    <t>first line for form 415, ie) tankless water heater, AC packaged unit (no suctions), new cabinets, new sink, new toilet</t>
+  </si>
+  <si>
+    <t>descr_of_work2</t>
+  </si>
+  <si>
+    <t>siding, drywall, 2x6 pier support setdown</t>
+  </si>
+  <si>
+    <t>2nd line for fomr 415, ie) siding, drywall, 2x6 pier support setdown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;Av&quot;\ #"/>
+    <numFmt numFmtId="165" formatCode="&quot;Al&quot;\ #"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,13 +341,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -234,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -253,6 +409,43 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,31 +760,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3EEFF51-2E49-41C8-A9EE-073E0BCFAF77}">
-  <dimension ref="B1:E28"/>
+  <dimension ref="B1:N72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.54296875" customWidth="1"/>
-    <col min="2" max="2" width="4.453125" customWidth="1"/>
-    <col min="3" max="3" width="14.90625" customWidth="1"/>
-    <col min="4" max="4" width="38.453125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="1.5703125" customWidth="1"/>
+    <col min="2" max="2" width="4.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -603,256 +796,532 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>14</v>
+      <c r="D4" t="s">
+        <v>66</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="N4" s="19"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="7">
         <v>2</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>33</v>
+      <c r="D5" s="22" t="s">
+        <v>67</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+      <c r="N5" s="20"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
+        <v>68</v>
+      </c>
+      <c r="N6" s="20"/>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="N7" s="19"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="4">
-        <v>1028239</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+      <c r="N8" s="19"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>42</v>
+      <c r="D9" t="s">
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+      <c r="N9" s="19"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="7">
         <v>7</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>17</v>
+      <c r="D10" t="s">
+        <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="7">
         <v>8</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>18</v>
+      <c r="D11" t="s">
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="N11" s="19"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="7">
         <v>9</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>34</v>
+      <c r="D12" s="22" t="s">
+        <v>65</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="N12" s="20"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>48</v>
+      </c>
+      <c r="N13" s="19"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="D14">
+        <v>24</v>
+      </c>
+      <c r="N14" s="19"/>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
       </c>
       <c r="E15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="N15" s="19"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>27</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D18" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B20">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="8">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B21">
+      <c r="C20" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="8">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B22">
+      <c r="C21" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="8">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C22" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>25</v>
       </c>
+    </row>
+    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>60</v>
+      </c>
+      <c r="H37" t="s">
+        <v>57</v>
+      </c>
+      <c r="J37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>42</v>
+      </c>
+      <c r="H38" t="s">
+        <v>48</v>
+      </c>
+      <c r="J38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
+        <v>58</v>
+      </c>
+      <c r="H39" t="s">
+        <v>53</v>
+      </c>
+      <c r="J39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
+        <v>43</v>
+      </c>
+      <c r="H40" t="s">
+        <v>49</v>
+      </c>
+      <c r="J40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D41" s="10"/>
+      <c r="F41" t="s">
+        <v>44</v>
+      </c>
+      <c r="H41" t="s">
+        <v>50</v>
+      </c>
+      <c r="J41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
+        <v>45</v>
+      </c>
+      <c r="H42" t="s">
+        <v>51</v>
+      </c>
+      <c r="J42">
+        <v>15244</v>
+      </c>
+    </row>
+    <row r="43" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D43" s="11"/>
+      <c r="F43" t="s">
+        <v>59</v>
+      </c>
+      <c r="H43" t="s">
+        <v>54</v>
+      </c>
+      <c r="J43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D44" s="12"/>
+      <c r="F44" t="s">
+        <v>47</v>
+      </c>
+      <c r="H44" t="s">
+        <v>47</v>
+      </c>
+      <c r="J44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D45" s="12"/>
+      <c r="F45" t="s">
+        <v>55</v>
+      </c>
+      <c r="H45" t="s">
+        <v>55</v>
+      </c>
+      <c r="J45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D46" s="13"/>
+      <c r="F46" t="s">
+        <v>56</v>
+      </c>
+      <c r="H46" t="s">
+        <v>56</v>
+      </c>
+      <c r="J46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D47" s="13"/>
+      <c r="F47">
+        <v>55</v>
+      </c>
+      <c r="H47">
+        <v>60</v>
+      </c>
+      <c r="J47">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D48" s="13"/>
+      <c r="F48">
+        <v>12</v>
+      </c>
+      <c r="H48">
+        <v>12</v>
+      </c>
+      <c r="J48">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D49" s="12"/>
+      <c r="F49" t="s">
+        <v>46</v>
+      </c>
+      <c r="H49" t="s">
+        <v>46</v>
+      </c>
+      <c r="J49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D50" s="12"/>
+      <c r="J50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D52" s="15"/>
+    </row>
+    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D53" s="16"/>
+    </row>
+    <row r="54" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D54" s="17"/>
+    </row>
+    <row r="55" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D55" s="16"/>
+    </row>
+    <row r="56" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D56" s="16"/>
+    </row>
+    <row r="57" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D57" s="16"/>
+    </row>
+    <row r="58" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D58" s="16"/>
+    </row>
+    <row r="59" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D59" s="16"/>
+    </row>
+    <row r="60" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D60" s="18"/>
+    </row>
+    <row r="61" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D61" s="18"/>
+    </row>
+    <row r="63" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D63" s="14"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="11"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="12"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="12"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="13"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D69" s="13"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D70" s="13"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D71"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D72" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>